<commit_message>
Revert "Login page construction"
This reverts commit 1d61e25ccc609ede6906f5d03992c54499fc5e3a.
</commit_message>
<xml_diff>
--- a/Instagram 기획안.xlsx
+++ b/Instagram 기획안.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iiuuy\Documents\Instagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iiuuy\바탕 화면\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09A746D-0802-4DE6-B035-278C250F1441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C432F9-A5A6-459C-A016-2AD985C2E54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4734D3AC-BB1E-4202-81B8-23CF3B3C6E37}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -230,206 +230,6 @@
   </si>
   <si>
     <t>가입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>레스토랑 프로젝트 마무리</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">예희 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>postman 으로는 삭제 O -&gt; 삭제 버튼 -&gt; 삭제 X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">오류 : </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이것만 하면 끝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예약번호 찾기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>where 이름, 전화 -&gt; 예약번호를 가져와라</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>확인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고객님의 예약번호는 ㅁㅁㅁ 입니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>confirm -&gt; window(자식창)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아셀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터 insert 까지 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제로 금액값이 안넘어감 (1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제 후 DB insert (2)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null -&gt; 해결</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정은</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no image, 관리자예약조회 -&gt; null, undefine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자 로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>현경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>main</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 문제 : 데이터를 innertext불러옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;- 버튼 toggle 이 안됨(js)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>데이터가 불러와지는게, console이랑 postman으로는 확인이됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그런데, 메뉴 div list에는 어떻게 불러와지는지 확인안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예약 변경</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>페이지 구성은 완료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data null 로 불러와짐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consol로는 데이터가 가져와짐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update 구현 안됨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>23.3.23 추가</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>controller 매핑 안되어있음 ㅎ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>23.03.23 + 예약 확인페이지 -&gt; 예약변경 -&gt; 예약 변경 페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추가 병합시 오류 head 수정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인기능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SNS 로그인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입 - ROLEMST 권한 USER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스크롤시 -&gt;좌우로 넘어가도록 구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>참고사이트 : 포스타입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기능 : 좋아요, 댓글, DM, 저장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>댓글 -&gt; 좋아요?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NEW WINDOW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시물 좌우 버튼 -&gt; 로드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>좌측 목록에서 프로필을 누르면 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>팔로워, 팔로우</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>COUNT 게시물수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>게시글 쓰기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>삭제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -437,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,22 +273,6 @@
       <name val="HY견명조"/>
       <family val="1"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="26"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -535,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -686,65 +470,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -901,34 +633,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -943,14 +651,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,8 +699,8 @@
       <xdr:rowOff>22861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>7621</xdr:rowOff>
     </xdr:to>
@@ -1600,59 +1320,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>205740</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="직선 화살표 연결선 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C7A7BC-B8BF-7011-689F-EC803D90C22E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8633460" y="19583400"/>
-          <a:ext cx="1333500" cy="167640"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1955,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312320AA-781C-4489-9CA8-99AE3B64EE9C}">
   <dimension ref="A3:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1965,19 +1632,19 @@
     <col min="2" max="2" width="8.796875" style="1"/>
     <col min="3" max="3" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.796875" style="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.296875" style="1" customWidth="1"/>
     <col min="6" max="13" width="8.796875" style="1"/>
     <col min="14" max="16" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="59" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1985,7 +1652,7 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="59" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3"/>
@@ -1994,7 +1661,7 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="59" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="6"/>
@@ -2009,7 +1676,7 @@
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="59" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="6"/>
@@ -2037,10 +1704,10 @@
         <v>2</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="53"/>
+      <c r="K8" s="58"/>
       <c r="L8" s="8" t="s">
         <v>8</v>
       </c>
@@ -2048,32 +1715,29 @@
     </row>
     <row r="9" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F9" s="6"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="7"/>
-      <c r="L9" s="62" t="s">
+      <c r="L9" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="M9" s="63"/>
+      <c r="M9" s="55"/>
     </row>
     <row r="10" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F10" s="6"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F11" s="6"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F12" s="6"/>
       <c r="I12" s="7"/>
-      <c r="L12" s="1" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="13" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F13" s="8"/>
@@ -2081,30 +1745,18 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F14" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F15" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F16" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="55" t="s">
+    <row r="14" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="56"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
@@ -2119,93 +1771,50 @@
       </c>
       <c r="M21" s="2"/>
       <c r="P21"/>
-      <c r="Q21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C22" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="5"/>
+    </row>
+    <row r="22" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E22" s="16"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="18"/>
       <c r="M22" s="2"/>
       <c r="P22"/>
-      <c r="Q22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="7"/>
+    </row>
+    <row r="23" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="21"/>
       <c r="M23" s="2"/>
       <c r="P23"/>
-      <c r="Q23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="7"/>
+    </row>
+    <row r="24" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
-      <c r="L24" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="M24" s="2"/>
       <c r="P24"/>
     </row>
-    <row r="25" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="7"/>
+    <row r="25" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E25" s="19"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="21"/>
-      <c r="L25" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="7"/>
+    </row>
+    <row r="26" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C27" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="7"/>
+    <row r="27" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C28" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="10"/>
+    <row r="28" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E28" s="6"/>
       <c r="F28" s="1" t="s">
         <v>13</v>
@@ -2214,12 +1823,8 @@
         <v>14</v>
       </c>
       <c r="H28" s="7"/>
-      <c r="J28" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C29"/>
+    </row>
+    <row r="29" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E29" s="6" t="s">
         <v>15</v>
       </c>
@@ -2227,20 +1832,12 @@
         <v>16</v>
       </c>
       <c r="H29" s="7"/>
-      <c r="J29" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C30"/>
+    </row>
+    <row r="30" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E30" s="6"/>
       <c r="H30" s="7"/>
-      <c r="J30" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C31"/>
+    </row>
+    <row r="31" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E31" s="8" t="s">
         <v>17</v>
       </c>
@@ -2248,7 +1845,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="3:18" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="34" spans="3:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F34" s="28"/>
@@ -2299,9 +1896,6 @@
       <c r="L37" s="25"/>
       <c r="M37" s="26"/>
       <c r="N37"/>
-      <c r="O37" s="2" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="38" spans="3:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F38" s="32"/>
@@ -2313,15 +1907,12 @@
       <c r="L38"/>
       <c r="M38" s="27"/>
       <c r="N38"/>
-      <c r="O38" s="2" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="39" spans="3:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
@@ -2370,12 +1961,10 @@
     <row r="43" spans="3:18" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="3:18" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="45" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="57" t="s">
+      <c r="C45" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D45" t="s">
-        <v>93</v>
-      </c>
+      <c r="D45"/>
       <c r="E45"/>
       <c r="F45"/>
       <c r="G45"/>
@@ -2396,12 +1985,9 @@
       <c r="F46"/>
       <c r="G46"/>
       <c r="H46"/>
-      <c r="I46" t="s">
-        <v>95</v>
-      </c>
-      <c r="K46" t="s">
-        <v>94</v>
-      </c>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
@@ -2409,11 +1995,11 @@
       <c r="P46"/>
     </row>
     <row r="47" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C47" s="47" t="s">
+      <c r="C47" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="25"/>
-      <c r="E47" s="26"/>
+      <c r="D47"/>
+      <c r="E47"/>
       <c r="F47" s="47"/>
       <c r="G47" s="25"/>
       <c r="H47" s="25" t="s">
@@ -2428,7 +2014,7 @@
       <c r="K47" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L47" s="68" t="s">
+      <c r="L47" s="52" t="s">
         <v>39</v>
       </c>
       <c r="M47" s="26" t="s">
@@ -2441,11 +2027,11 @@
       <c r="P47"/>
     </row>
     <row r="48" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C48" s="48" t="s">
+      <c r="C48" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="67"/>
-      <c r="E48" s="27"/>
+      <c r="D48"/>
+      <c r="E48"/>
       <c r="F48" s="48"/>
       <c r="G48"/>
       <c r="H48"/>
@@ -2455,7 +2041,7 @@
       <c r="L48"/>
       <c r="M48" s="27"/>
       <c r="N48"/>
-      <c r="O48" s="52" t="s">
+      <c r="O48" s="53" t="s">
         <v>29</v>
       </c>
       <c r="P48" s="37"/>
@@ -2463,11 +2049,11 @@
       <c r="R48" s="38"/>
     </row>
     <row r="49" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C49" s="48" t="s">
+      <c r="C49" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="67"/>
-      <c r="E49" s="27"/>
+      <c r="D49"/>
+      <c r="E49"/>
       <c r="F49" s="49"/>
       <c r="G49" s="50"/>
       <c r="H49" s="50"/>
@@ -2477,7 +2063,7 @@
       <c r="L49" s="50"/>
       <c r="M49" s="51"/>
       <c r="N49"/>
-      <c r="O49" s="52" t="s">
+      <c r="O49" s="53" t="s">
         <v>30</v>
       </c>
       <c r="P49" s="37"/>
@@ -2485,12 +2071,12 @@
       <c r="R49" s="38"/>
     </row>
     <row r="50" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C50" s="48" t="s">
+      <c r="C50" t="s">
         <v>23</v>
       </c>
-      <c r="D50" s="67"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="52"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50" s="53"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="37" t="s">
@@ -2505,7 +2091,7 @@
       <c r="L50" s="37"/>
       <c r="M50" s="38"/>
       <c r="N50"/>
-      <c r="O50" s="52" t="s">
+      <c r="O50" s="53" t="s">
         <v>31</v>
       </c>
       <c r="P50" s="37"/>
@@ -2513,11 +2099,11 @@
       <c r="R50" s="38"/>
     </row>
     <row r="51" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C51" s="48" t="s">
+      <c r="C51" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="67"/>
-      <c r="E51" s="27"/>
+      <c r="D51"/>
+      <c r="E51"/>
       <c r="F51" s="47"/>
       <c r="G51" s="25"/>
       <c r="H51" s="25"/>
@@ -2527,7 +2113,7 @@
       <c r="L51" s="25"/>
       <c r="M51" s="26"/>
       <c r="N51"/>
-      <c r="O51" s="52" t="s">
+      <c r="O51" s="53" t="s">
         <v>32</v>
       </c>
       <c r="P51" s="37"/>
@@ -2535,11 +2121,11 @@
       <c r="R51" s="38"/>
     </row>
     <row r="52" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C52" s="48" t="s">
+      <c r="C52" t="s">
         <v>25</v>
       </c>
-      <c r="D52" s="67"/>
-      <c r="E52" s="27"/>
+      <c r="D52"/>
+      <c r="E52"/>
       <c r="F52" s="48"/>
       <c r="G52"/>
       <c r="H52"/>
@@ -2549,7 +2135,7 @@
       <c r="L52"/>
       <c r="M52" s="27"/>
       <c r="N52"/>
-      <c r="O52" s="52" t="s">
+      <c r="O52" s="53" t="s">
         <v>33</v>
       </c>
       <c r="P52" s="37"/>
@@ -2557,11 +2143,11 @@
       <c r="R52" s="38"/>
     </row>
     <row r="53" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C53" s="48" t="s">
+      <c r="C53" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="67"/>
-      <c r="E53" s="27"/>
+      <c r="D53"/>
+      <c r="E53"/>
       <c r="F53" s="48"/>
       <c r="G53"/>
       <c r="H53"/>
@@ -2571,7 +2157,7 @@
       <c r="L53"/>
       <c r="M53" s="27"/>
       <c r="N53"/>
-      <c r="O53" s="52" t="s">
+      <c r="O53" s="53" t="s">
         <v>34</v>
       </c>
       <c r="P53" s="37"/>
@@ -2579,9 +2165,9 @@
       <c r="R53" s="38"/>
     </row>
     <row r="54" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C54" s="48"/>
-      <c r="D54" s="67"/>
-      <c r="E54" s="27"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
       <c r="F54" s="48"/>
       <c r="G54"/>
       <c r="H54"/>
@@ -2591,7 +2177,7 @@
       <c r="L54"/>
       <c r="M54" s="27"/>
       <c r="N54"/>
-      <c r="O54" s="52" t="s">
+      <c r="O54" s="53" t="s">
         <v>35</v>
       </c>
       <c r="P54" s="37"/>
@@ -2599,9 +2185,9 @@
       <c r="R54" s="38"/>
     </row>
     <row r="55" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C55" s="48"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="27"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
       <c r="F55" s="48"/>
       <c r="G55"/>
       <c r="H55"/>
@@ -2617,9 +2203,9 @@
       <c r="P55"/>
     </row>
     <row r="56" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="51"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
       <c r="F56" s="49"/>
       <c r="G56" s="50"/>
       <c r="H56" s="50"/>
@@ -2675,261 +2261,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83937A6-931B-4FF1-88D3-EB44579043AD}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A2:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.796875" customWidth="1"/>
-    <col min="5" max="5" width="8.796875" customWidth="1"/>
-    <col min="6" max="6" width="3.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A1" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-    </row>
-    <row r="2" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-    </row>
-    <row r="3" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="61" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="26"/>
-    </row>
-    <row r="9" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="48"/>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="I9" s="48"/>
-      <c r="J9" t="s">
-        <v>57</v>
-      </c>
-      <c r="N9" s="27"/>
-    </row>
-    <row r="10" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="48"/>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="27"/>
-      <c r="I10" s="48"/>
-      <c r="N10" s="27"/>
-    </row>
-    <row r="11" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="48"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="27"/>
-      <c r="I11" s="48"/>
-      <c r="M11" t="s">
-        <v>56</v>
-      </c>
-      <c r="N11" s="27"/>
-    </row>
-    <row r="12" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="49"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="51"/>
-    </row>
-    <row r="13" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="58"/>
-    </row>
-    <row r="24" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C24" s="48"/>
-      <c r="F24" s="59"/>
-      <c r="G24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="48"/>
-      <c r="F25" s="59"/>
-      <c r="G25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="60"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C33" t="s">
-        <v>77</v>
-      </c>
-    </row>
+    <row r="2" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="3" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="4" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="5" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="6" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="7" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="8" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="10" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="11" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="12" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="13" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="15" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="17" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="22" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="24" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="25" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J2"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Login page construction""
This reverts commit 9fec455dc627dd8e679ab74a5fb20264ea82aa1d.
</commit_message>
<xml_diff>
--- a/Instagram 기획안.xlsx
+++ b/Instagram 기획안.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iiuuy\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iiuuy\Documents\Instagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C432F9-A5A6-459C-A016-2AD985C2E54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09A746D-0802-4DE6-B035-278C250F1441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4734D3AC-BB1E-4202-81B8-23CF3B3C6E37}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
   <si>
     <t>로그인</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -230,6 +230,206 @@
   </si>
   <si>
     <t>가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레스토랑 프로젝트 마무리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">예희 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>postman 으로는 삭제 O -&gt; 삭제 버튼 -&gt; 삭제 X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">오류 : </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이것만 하면 끝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약번호 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>where 이름, 전화 -&gt; 예약번호를 가져와라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고객님의 예약번호는 ㅁㅁㅁ 입니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>confirm -&gt; window(자식창)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아셀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 insert 까지 완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제로 금액값이 안넘어감 (1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제 후 DB insert (2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null -&gt; 해결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no image, 관리자예약조회 -&gt; null, undefine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자 로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>main</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 문제 : 데이터를 innertext불러옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;- 버튼 toggle 이 안됨(js)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터가 불러와지는게, console이랑 postman으로는 확인이됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그런데, 메뉴 div list에는 어떻게 불러와지는지 확인안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예약 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이지 구성은 완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data null 로 불러와짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>consol로는 데이터가 가져와짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update 구현 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23.3.23 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller 매핑 안되어있음 ㅎ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23.03.23 + 예약 확인페이지 -&gt; 예약변경 -&gt; 예약 변경 페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>추가 병합시 오류 head 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNS 로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 - ROLEMST 권한 USER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스크롤시 -&gt;좌우로 넘어가도록 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>참고사이트 : 포스타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 : 좋아요, 댓글, DM, 저장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>댓글 -&gt; 좋아요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEW WINDOW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시물 좌우 버튼 -&gt; 로드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좌측 목록에서 프로필을 누르면 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔로워, 팔로우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>COUNT 게시물수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 쓰기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -237,7 +437,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +473,22 @@
       <name val="HY견명조"/>
       <family val="1"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -319,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -470,13 +686,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -633,10 +901,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -651,26 +943,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,8 +979,8 @@
       <xdr:rowOff>22861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>7621</xdr:rowOff>
     </xdr:to>
@@ -1320,6 +1600,59 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="직선 화살표 연결선 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C7A7BC-B8BF-7011-689F-EC803D90C22E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8633460" y="19583400"/>
+          <a:ext cx="1333500" cy="167640"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1622,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312320AA-781C-4489-9CA8-99AE3B64EE9C}">
   <dimension ref="A3:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1632,19 +1965,19 @@
     <col min="2" max="2" width="8.796875" style="1"/>
     <col min="3" max="3" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.796875" style="1"/>
-    <col min="5" max="5" width="6.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
     <col min="6" max="13" width="8.796875" style="1"/>
     <col min="14" max="16" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="54" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1652,7 +1985,7 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="54" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="3"/>
@@ -1661,7 +1994,7 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="54" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="6"/>
@@ -1676,7 +2009,7 @@
       <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="54" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="6"/>
@@ -1704,10 +2037,10 @@
         <v>2</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="58" t="s">
+      <c r="J8" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="58"/>
+      <c r="K8" s="53"/>
       <c r="L8" s="8" t="s">
         <v>8</v>
       </c>
@@ -1715,29 +2048,32 @@
     </row>
     <row r="9" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F9" s="6"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="57"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="7"/>
-      <c r="L9" s="54" t="s">
+      <c r="L9" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="M9" s="55"/>
+      <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F10" s="6"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="57"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="65"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:13" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F11" s="6"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="57"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F12" s="6"/>
       <c r="I12" s="7"/>
+      <c r="L12" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F13" s="8"/>
@@ -1745,18 +2081,30 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="60" t="s">
+    <row r="14" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F15" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="25.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F16" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="61"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1771,50 +2119,93 @@
       </c>
       <c r="M21" s="2"/>
       <c r="P21"/>
-    </row>
-    <row r="22" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C22" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="16"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="18"/>
       <c r="M22" s="2"/>
       <c r="P22"/>
-    </row>
-    <row r="23" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C23" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="21"/>
       <c r="M23" s="2"/>
       <c r="P23"/>
-    </row>
-    <row r="24" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="Q23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C24" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="7"/>
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
+      <c r="L24" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="M24" s="2"/>
       <c r="P24"/>
     </row>
-    <row r="25" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="7"/>
       <c r="E25" s="19"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="L25" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="7"/>
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
     </row>
-    <row r="27" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C27" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="7"/>
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C28" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="10"/>
       <c r="E28" s="6"/>
       <c r="F28" s="1" t="s">
         <v>13</v>
@@ -1823,8 +2214,12 @@
         <v>14</v>
       </c>
       <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J28" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C29"/>
       <c r="E29" s="6" t="s">
         <v>15</v>
       </c>
@@ -1832,12 +2227,20 @@
         <v>16</v>
       </c>
       <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J29" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C30"/>
       <c r="E30" s="6"/>
       <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:16" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J30" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C31"/>
       <c r="E31" s="8" t="s">
         <v>17</v>
       </c>
@@ -1845,7 +2248,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="10"/>
     </row>
-    <row r="32" spans="1:16" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="32" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="3:18" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="34" spans="3:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F34" s="28"/>
@@ -1896,6 +2299,9 @@
       <c r="L37" s="25"/>
       <c r="M37" s="26"/>
       <c r="N37"/>
+      <c r="O37" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="38" spans="3:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="F38" s="32"/>
@@ -1907,12 +2313,15 @@
       <c r="L38"/>
       <c r="M38" s="27"/>
       <c r="N38"/>
+      <c r="O38" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="39" spans="3:18" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="F39" s="62"/>
-      <c r="G39" s="62"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="63"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
@@ -1961,10 +2370,12 @@
     <row r="43" spans="3:18" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="3:18" ht="54" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="45" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C45" s="64" t="s">
+      <c r="C45" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D45"/>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
       <c r="E45"/>
       <c r="F45"/>
       <c r="G45"/>
@@ -1985,9 +2396,12 @@
       <c r="F46"/>
       <c r="G46"/>
       <c r="H46"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
+      <c r="I46" t="s">
+        <v>95</v>
+      </c>
+      <c r="K46" t="s">
+        <v>94</v>
+      </c>
       <c r="L46"/>
       <c r="M46"/>
       <c r="N46"/>
@@ -1995,11 +2409,11 @@
       <c r="P46"/>
     </row>
     <row r="47" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C47" t="s">
+      <c r="C47" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D47"/>
-      <c r="E47"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="26"/>
       <c r="F47" s="47"/>
       <c r="G47" s="25"/>
       <c r="H47" s="25" t="s">
@@ -2014,7 +2428,7 @@
       <c r="K47" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="L47" s="52" t="s">
+      <c r="L47" s="68" t="s">
         <v>39</v>
       </c>
       <c r="M47" s="26" t="s">
@@ -2027,11 +2441,11 @@
       <c r="P47"/>
     </row>
     <row r="48" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C48" t="s">
+      <c r="C48" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D48"/>
-      <c r="E48"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="27"/>
       <c r="F48" s="48"/>
       <c r="G48"/>
       <c r="H48"/>
@@ -2041,7 +2455,7 @@
       <c r="L48"/>
       <c r="M48" s="27"/>
       <c r="N48"/>
-      <c r="O48" s="53" t="s">
+      <c r="O48" s="52" t="s">
         <v>29</v>
       </c>
       <c r="P48" s="37"/>
@@ -2049,11 +2463,11 @@
       <c r="R48" s="38"/>
     </row>
     <row r="49" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C49" t="s">
+      <c r="C49" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="D49"/>
-      <c r="E49"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="27"/>
       <c r="F49" s="49"/>
       <c r="G49" s="50"/>
       <c r="H49" s="50"/>
@@ -2063,7 +2477,7 @@
       <c r="L49" s="50"/>
       <c r="M49" s="51"/>
       <c r="N49"/>
-      <c r="O49" s="53" t="s">
+      <c r="O49" s="52" t="s">
         <v>30</v>
       </c>
       <c r="P49" s="37"/>
@@ -2071,12 +2485,12 @@
       <c r="R49" s="38"/>
     </row>
     <row r="50" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C50" t="s">
+      <c r="C50" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50" s="53"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="52"/>
       <c r="G50" s="37"/>
       <c r="H50" s="37"/>
       <c r="I50" s="37" t="s">
@@ -2091,7 +2505,7 @@
       <c r="L50" s="37"/>
       <c r="M50" s="38"/>
       <c r="N50"/>
-      <c r="O50" s="53" t="s">
+      <c r="O50" s="52" t="s">
         <v>31</v>
       </c>
       <c r="P50" s="37"/>
@@ -2099,11 +2513,11 @@
       <c r="R50" s="38"/>
     </row>
     <row r="51" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C51" t="s">
+      <c r="C51" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="D51"/>
-      <c r="E51"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="47"/>
       <c r="G51" s="25"/>
       <c r="H51" s="25"/>
@@ -2113,7 +2527,7 @@
       <c r="L51" s="25"/>
       <c r="M51" s="26"/>
       <c r="N51"/>
-      <c r="O51" s="53" t="s">
+      <c r="O51" s="52" t="s">
         <v>32</v>
       </c>
       <c r="P51" s="37"/>
@@ -2121,11 +2535,11 @@
       <c r="R51" s="38"/>
     </row>
     <row r="52" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C52" t="s">
+      <c r="C52" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D52"/>
-      <c r="E52"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="27"/>
       <c r="F52" s="48"/>
       <c r="G52"/>
       <c r="H52"/>
@@ -2135,7 +2549,7 @@
       <c r="L52"/>
       <c r="M52" s="27"/>
       <c r="N52"/>
-      <c r="O52" s="53" t="s">
+      <c r="O52" s="52" t="s">
         <v>33</v>
       </c>
       <c r="P52" s="37"/>
@@ -2143,11 +2557,11 @@
       <c r="R52" s="38"/>
     </row>
     <row r="53" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C53" t="s">
+      <c r="C53" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D53"/>
-      <c r="E53"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="27"/>
       <c r="F53" s="48"/>
       <c r="G53"/>
       <c r="H53"/>
@@ -2157,7 +2571,7 @@
       <c r="L53"/>
       <c r="M53" s="27"/>
       <c r="N53"/>
-      <c r="O53" s="53" t="s">
+      <c r="O53" s="52" t="s">
         <v>34</v>
       </c>
       <c r="P53" s="37"/>
@@ -2165,9 +2579,9 @@
       <c r="R53" s="38"/>
     </row>
     <row r="54" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="67"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="48"/>
       <c r="G54"/>
       <c r="H54"/>
@@ -2177,7 +2591,7 @@
       <c r="L54"/>
       <c r="M54" s="27"/>
       <c r="N54"/>
-      <c r="O54" s="53" t="s">
+      <c r="O54" s="52" t="s">
         <v>35</v>
       </c>
       <c r="P54" s="37"/>
@@ -2185,9 +2599,9 @@
       <c r="R54" s="38"/>
     </row>
     <row r="55" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="67"/>
+      <c r="E55" s="27"/>
       <c r="F55" s="48"/>
       <c r="G55"/>
       <c r="H55"/>
@@ -2203,9 +2617,9 @@
       <c r="P55"/>
     </row>
     <row r="56" spans="3:18" ht="29.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="51"/>
       <c r="F56" s="49"/>
       <c r="G56" s="50"/>
       <c r="H56" s="50"/>
@@ -2261,42 +2675,261 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83937A6-931B-4FF1-88D3-EB44579043AD}">
-  <dimension ref="A2:A25"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.796875" customWidth="1"/>
+    <col min="5" max="5" width="8.796875" customWidth="1"/>
+    <col min="6" max="6" width="3.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="3" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="4" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="5" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="7" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="8" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="12" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="13" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="15" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="18" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A1" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+    </row>
+    <row r="2" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+    </row>
+    <row r="3" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="26"/>
+    </row>
+    <row r="9" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="48"/>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="I9" s="48"/>
+      <c r="J9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" s="27"/>
+    </row>
+    <row r="10" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="48"/>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="27"/>
+      <c r="I10" s="48"/>
+      <c r="N10" s="27"/>
+    </row>
+    <row r="11" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="48"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="I11" s="48"/>
+      <c r="M11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="27"/>
+    </row>
+    <row r="12" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="51"/>
+    </row>
+    <row r="13" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="58"/>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C24" s="48"/>
+      <c r="F24" s="59"/>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="48"/>
+      <c r="F25" s="59"/>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="60"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>